<commit_message>
update save path env variable
</commit_message>
<xml_diff>
--- a/doc/GCS_CASE.xlsx
+++ b/doc/GCS_CASE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zombies13/Desktop/Projects/GCS2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\dlt-components\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0693F16-0123-C94A-AE50-D2DE17399C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CFCECC-20F4-4CFB-9E07-1DB11C22C2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="500" windowWidth="34480" windowHeight="19780" xr2:uid="{1CFF61F2-10D9-4845-A355-67ECCC8ACF87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CFF61F2-10D9-4845-A355-67ECCC8ACF87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>CASE</t>
   </si>
@@ -45,9 +41,6 @@
   </si>
   <si>
     <t>Record</t>
-  </si>
-  <si>
-    <t>InCorrect</t>
   </si>
   <si>
     <t>OUT</t>
@@ -132,18 +125,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -152,13 +145,19 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -370,9 +369,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,7 +381,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -408,6 +405,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -417,30 +435,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -456,7 +467,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -752,384 +763,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0B36A3-9F6D-AA46-A37C-3425373A0C3A}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="8.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="4" customWidth="1"/>
-    <col min="7" max="8" width="8.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="91.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="91.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="F1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="22"/>
+      <c r="H1" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="18">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="12" t="s">
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="18">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="28" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A8" s="23">
+        <v>6</v>
+      </c>
+      <c r="B8" s="23">
+        <v>0</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+      <c r="F8" s="23"/>
+      <c r="G8" s="25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="12">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11">
-        <v>0</v>
-      </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="8">
-        <v>0</v>
-      </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14" t="s">
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="12">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="12">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="18">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="23">
-        <v>0</v>
-      </c>
-      <c r="I5" s="14">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="23">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="12">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="18">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="23">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="23">
-        <v>0</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>6</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="24">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="13">
-        <v>0</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>7</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14" t="s">
+      <c r="I13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="19">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="8">
-        <v>0</v>
-      </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="14">
-        <v>0</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="23">
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>11</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="23">
-        <v>0</v>
-      </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="I14" s="4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>12</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="13">
-        <v>0</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="24">
-        <v>0</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="13">
-        <v>0</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>